<commit_message>
excel file data modified to Pass all test cases
</commit_message>
<xml_diff>
--- a/testData/LoginData.xlsx
+++ b/testData/LoginData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="21" documentId="11_F25DC773A252ABEACE02ECEDDB99737E5ADE589E" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{AEC81229-D5BE-4C03-A75F-6CE8DDE39935}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A17D19-8225-4615-9570-287B2E041901}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2330" yWindow="2560" windowWidth="16870" windowHeight="7640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Invalid</t>
-  </si>
-  <si>
-    <t>iifEL1</t>
   </si>
 </sst>
 </file>
@@ -466,7 +463,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>7</v>

</xml_diff>